<commit_message>
adding models and routes
</commit_message>
<xml_diff>
--- a/E-commerce.xlsx
+++ b/E-commerce.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\CRISTIAN\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\CRISTIAN\Desktop\E-commerce_project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AB1BFC66-D8BD-4E8D-A0FA-E309334A7229}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8D536502-C9EF-450A-8A5C-5D1A4020F214}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="19440" windowHeight="15000" activeTab="3" xr2:uid="{31B28896-3896-40FF-81CA-A0B12D40E57B}"/>
   </bookViews>
@@ -16,7 +16,7 @@
     <sheet name="main" sheetId="1" r:id="rId1"/>
     <sheet name="vistas" sheetId="3" r:id="rId2"/>
     <sheet name="Modelado" sheetId="2" r:id="rId3"/>
-    <sheet name="Relaciones" sheetId="4" r:id="rId4"/>
+    <sheet name="Relaciones_SQL" sheetId="4" r:id="rId4"/>
     <sheet name="Reglas_negocio" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="191029"/>
@@ -1051,6 +1051,23 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="20" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1122,23 +1139,6 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="20" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -2475,18 +2475,18 @@
       </c>
       <c r="V3" s="10"/>
       <c r="X3" s="8"/>
-      <c r="Y3" s="41" t="s">
+      <c r="Y3" s="50" t="s">
         <v>82</v>
       </c>
-      <c r="Z3" s="42"/>
-      <c r="AA3" s="43"/>
+      <c r="Z3" s="51"/>
+      <c r="AA3" s="52"/>
       <c r="AB3" s="10"/>
       <c r="AD3" s="8"/>
-      <c r="AE3" s="50" t="s">
+      <c r="AE3" s="59" t="s">
         <v>82</v>
       </c>
-      <c r="AF3" s="51"/>
-      <c r="AG3" s="52"/>
+      <c r="AF3" s="60"/>
+      <c r="AG3" s="61"/>
       <c r="AH3" s="10"/>
     </row>
     <row r="4" spans="1:34" x14ac:dyDescent="0.25">
@@ -2524,14 +2524,14 @@
       </c>
       <c r="V4" s="10"/>
       <c r="X4" s="8"/>
-      <c r="Y4" s="47"/>
-      <c r="Z4" s="48"/>
-      <c r="AA4" s="49"/>
+      <c r="Y4" s="56"/>
+      <c r="Z4" s="57"/>
+      <c r="AA4" s="58"/>
       <c r="AB4" s="10"/>
       <c r="AD4" s="8"/>
-      <c r="AE4" s="53"/>
-      <c r="AF4" s="54"/>
-      <c r="AG4" s="55"/>
+      <c r="AE4" s="62"/>
+      <c r="AF4" s="63"/>
+      <c r="AG4" s="64"/>
       <c r="AH4" s="10"/>
     </row>
     <row r="5" spans="1:34" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -2565,14 +2565,14 @@
       </c>
       <c r="V5" s="10"/>
       <c r="X5" s="8"/>
-      <c r="Y5" s="47"/>
-      <c r="Z5" s="48"/>
-      <c r="AA5" s="49"/>
+      <c r="Y5" s="56"/>
+      <c r="Z5" s="57"/>
+      <c r="AA5" s="58"/>
       <c r="AB5" s="10"/>
       <c r="AD5" s="8"/>
-      <c r="AE5" s="56"/>
-      <c r="AF5" s="57"/>
-      <c r="AG5" s="58"/>
+      <c r="AE5" s="65"/>
+      <c r="AF5" s="66"/>
+      <c r="AG5" s="67"/>
       <c r="AH5" s="10"/>
     </row>
     <row r="6" spans="1:34" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -2598,9 +2598,9 @@
       </c>
       <c r="V6" s="10"/>
       <c r="X6" s="8"/>
-      <c r="Y6" s="44"/>
-      <c r="Z6" s="45"/>
-      <c r="AA6" s="46"/>
+      <c r="Y6" s="53"/>
+      <c r="Z6" s="54"/>
+      <c r="AA6" s="55"/>
       <c r="AB6" s="10"/>
       <c r="AD6" s="8"/>
       <c r="AE6" s="9"/>
@@ -3209,11 +3209,11 @@
         <v>1</v>
       </c>
       <c r="X19" s="8"/>
-      <c r="Y19" s="41" t="s">
+      <c r="Y19" s="50" t="s">
         <v>81</v>
       </c>
-      <c r="Z19" s="42"/>
-      <c r="AA19" s="43"/>
+      <c r="Z19" s="51"/>
+      <c r="AA19" s="52"/>
       <c r="AB19" s="10"/>
       <c r="AD19" s="8"/>
       <c r="AE19" s="9" t="s">
@@ -3256,9 +3256,9 @@
       </c>
       <c r="V20" s="7"/>
       <c r="X20" s="8"/>
-      <c r="Y20" s="44"/>
-      <c r="Z20" s="45"/>
-      <c r="AA20" s="46"/>
+      <c r="Y20" s="53"/>
+      <c r="Z20" s="54"/>
+      <c r="AA20" s="55"/>
       <c r="AB20" s="10"/>
       <c r="AD20" s="8"/>
       <c r="AE20" s="5"/>
@@ -3512,11 +3512,11 @@
       <c r="AA27" s="9"/>
       <c r="AB27" s="10"/>
       <c r="AD27" s="8"/>
-      <c r="AE27" s="59" t="s">
+      <c r="AE27" s="68" t="s">
         <v>87</v>
       </c>
-      <c r="AF27" s="60"/>
-      <c r="AG27" s="61"/>
+      <c r="AF27" s="69"/>
+      <c r="AG27" s="70"/>
       <c r="AH27" s="10"/>
     </row>
     <row r="28" spans="1:34" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -3618,13 +3618,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="24" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="62" t="s">
+      <c r="A1" s="71" t="s">
         <v>23</v>
       </c>
-      <c r="B1" s="63"/>
-      <c r="C1" s="63"/>
-      <c r="D1" s="63"/>
-      <c r="E1" s="64"/>
+      <c r="B1" s="72"/>
+      <c r="C1" s="72"/>
+      <c r="D1" s="72"/>
+      <c r="E1" s="73"/>
     </row>
     <row r="2" spans="1:5" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="36" t="s">
@@ -4213,7 +4213,7 @@
       <c r="E49" s="10"/>
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A50" s="71" t="s">
+      <c r="A50" s="47" t="s">
         <v>184</v>
       </c>
       <c r="B50" s="30" t="s">
@@ -4250,7 +4250,7 @@
       <c r="E52" s="13"/>
     </row>
     <row r="53" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A53" s="71" t="s">
+      <c r="A53" s="47" t="s">
         <v>183</v>
       </c>
       <c r="B53" s="30" t="s">
@@ -4287,7 +4287,7 @@
       <c r="E55" s="13"/>
     </row>
     <row r="56" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A56" s="71" t="s">
+      <c r="A56" s="47" t="s">
         <v>187</v>
       </c>
       <c r="B56" s="30" t="s">
@@ -4324,7 +4324,7 @@
       <c r="E58" s="13"/>
     </row>
     <row r="59" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A59" s="71" t="s">
+      <c r="A59" s="47" t="s">
         <v>205</v>
       </c>
       <c r="B59" s="30" t="s">
@@ -4377,7 +4377,7 @@
   <dimension ref="B2:J45"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="H20" sqref="H20"/>
+      <selection activeCell="J19" sqref="J19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4394,13 +4394,13 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="H2" s="66" t="s">
+      <c r="H2" s="42" t="s">
         <v>171</v>
       </c>
-      <c r="I2" s="66" t="s">
+      <c r="I2" s="42" t="s">
         <v>172</v>
       </c>
-      <c r="J2" s="66" t="s">
+      <c r="J2" s="42" t="s">
         <v>170</v>
       </c>
     </row>
@@ -4408,13 +4408,13 @@
       <c r="B3" s="38" t="s">
         <v>62</v>
       </c>
-      <c r="H3" s="67" t="s">
+      <c r="H3" s="43" t="s">
         <v>173</v>
       </c>
-      <c r="I3" s="67" t="s">
+      <c r="I3" s="43" t="s">
         <v>89</v>
       </c>
-      <c r="J3" s="67" t="s">
+      <c r="J3" s="43" t="s">
         <v>168</v>
       </c>
     </row>
@@ -4425,13 +4425,13 @@
       <c r="D4" s="38" t="s">
         <v>89</v>
       </c>
-      <c r="H4" s="67" t="s">
+      <c r="H4" s="43" t="s">
         <v>173</v>
       </c>
-      <c r="I4" s="67" t="s">
+      <c r="I4" s="43" t="s">
         <v>55</v>
       </c>
-      <c r="J4" s="70" t="s">
+      <c r="J4" s="46" t="s">
         <v>168</v>
       </c>
     </row>
@@ -4442,13 +4442,13 @@
       <c r="D5" s="14" t="s">
         <v>147</v>
       </c>
-      <c r="H5" s="67" t="s">
+      <c r="H5" s="43" t="s">
         <v>96</v>
       </c>
-      <c r="I5" s="67" t="s">
+      <c r="I5" s="43" t="s">
         <v>174</v>
       </c>
-      <c r="J5" s="69" t="s">
+      <c r="J5" s="45" t="s">
         <v>168</v>
       </c>
     </row>
@@ -4459,13 +4459,13 @@
       <c r="D6" s="14" t="s">
         <v>148</v>
       </c>
-      <c r="H6" s="67" t="s">
+      <c r="H6" s="43" t="s">
         <v>55</v>
       </c>
-      <c r="I6" s="68" t="s">
+      <c r="I6" s="44" t="s">
         <v>90</v>
       </c>
-      <c r="J6" s="67" t="s">
+      <c r="J6" s="43" t="s">
         <v>185</v>
       </c>
     </row>
@@ -4476,13 +4476,13 @@
       <c r="D7" s="14" t="s">
         <v>149</v>
       </c>
-      <c r="H7" s="67" t="s">
+      <c r="H7" s="43" t="s">
         <v>55</v>
       </c>
-      <c r="I7" s="67" t="s">
+      <c r="I7" s="43" t="s">
         <v>175</v>
       </c>
-      <c r="J7" s="67" t="s">
+      <c r="J7" s="43" t="s">
         <v>169</v>
       </c>
     </row>
@@ -4493,13 +4493,13 @@
       <c r="D8" s="14" t="s">
         <v>150</v>
       </c>
-      <c r="H8" s="67" t="s">
+      <c r="H8" s="43" t="s">
         <v>55</v>
       </c>
-      <c r="I8" s="67" t="s">
+      <c r="I8" s="43" t="s">
         <v>176</v>
       </c>
-      <c r="J8" s="67" t="s">
+      <c r="J8" s="43" t="s">
         <v>185</v>
       </c>
     </row>
@@ -4513,13 +4513,13 @@
       <c r="F9" s="38" t="s">
         <v>189</v>
       </c>
-      <c r="H9" s="67" t="s">
+      <c r="H9" s="43" t="s">
         <v>55</v>
       </c>
-      <c r="I9" s="67" t="s">
+      <c r="I9" s="43" t="s">
         <v>177</v>
       </c>
-      <c r="J9" s="67" t="s">
+      <c r="J9" s="43" t="s">
         <v>168</v>
       </c>
     </row>
@@ -4533,13 +4533,13 @@
       <c r="F10" s="14" t="s">
         <v>158</v>
       </c>
-      <c r="H10" s="67" t="s">
+      <c r="H10" s="43" t="s">
         <v>55</v>
       </c>
-      <c r="I10" s="67" t="s">
+      <c r="I10" s="43" t="s">
         <v>178</v>
       </c>
-      <c r="J10" s="67" t="s">
+      <c r="J10" s="43" t="s">
         <v>185</v>
       </c>
     </row>
@@ -4550,13 +4550,13 @@
       <c r="F11" s="39" t="s">
         <v>136</v>
       </c>
-      <c r="H11" s="67" t="s">
+      <c r="H11" s="43" t="s">
         <v>55</v>
       </c>
-      <c r="I11" s="67" t="s">
+      <c r="I11" s="43" t="s">
         <v>179</v>
       </c>
-      <c r="J11" s="67" t="s">
+      <c r="J11" s="43" t="s">
         <v>185</v>
       </c>
     </row>
@@ -4648,7 +4648,7 @@
       </c>
     </row>
     <row r="25" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B25" s="65" t="s">
+      <c r="B25" s="41" t="s">
         <v>184</v>
       </c>
     </row>
@@ -4674,7 +4674,7 @@
       </c>
     </row>
     <row r="29" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B29" s="65" t="s">
+      <c r="B29" s="41" t="s">
         <v>183</v>
       </c>
     </row>
@@ -4700,7 +4700,7 @@
       </c>
     </row>
     <row r="33" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B33" s="65" t="s">
+      <c r="B33" s="41" t="s">
         <v>187</v>
       </c>
     </row>
@@ -4726,7 +4726,7 @@
       </c>
     </row>
     <row r="37" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B37" s="65" t="s">
+      <c r="B37" s="41" t="s">
         <v>205</v>
       </c>
       <c r="F37" s="9"/>
@@ -4795,82 +4795,82 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" s="66" t="s">
+      <c r="A1" s="42" t="s">
         <v>171</v>
       </c>
-      <c r="B1" s="72" t="s">
+      <c r="B1" s="48" t="s">
         <v>201</v>
       </c>
     </row>
     <row r="2" spans="1:2" ht="75.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="67" t="s">
+      <c r="A2" s="43" t="s">
         <v>96</v>
       </c>
-      <c r="B2" s="73" t="s">
+      <c r="B2" s="49" t="s">
         <v>208</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="75" x14ac:dyDescent="0.25">
-      <c r="A3" s="67" t="s">
+      <c r="A3" s="43" t="s">
         <v>55</v>
       </c>
-      <c r="B3" s="73" t="s">
+      <c r="B3" s="49" t="s">
         <v>209</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="75" x14ac:dyDescent="0.25">
-      <c r="A4" s="67" t="s">
+      <c r="A4" s="43" t="s">
         <v>202</v>
       </c>
-      <c r="B4" s="73" t="s">
+      <c r="B4" s="49" t="s">
         <v>210</v>
       </c>
     </row>
     <row r="5" spans="1:2" ht="75" x14ac:dyDescent="0.25">
-      <c r="A5" s="67" t="s">
+      <c r="A5" s="43" t="s">
         <v>41</v>
       </c>
-      <c r="B5" s="73" t="s">
+      <c r="B5" s="49" t="s">
         <v>211</v>
       </c>
     </row>
     <row r="6" spans="1:2" ht="75" x14ac:dyDescent="0.25">
-      <c r="A6" s="67" t="s">
+      <c r="A6" s="43" t="s">
         <v>116</v>
       </c>
-      <c r="B6" s="73" t="s">
+      <c r="B6" s="49" t="s">
         <v>212</v>
       </c>
     </row>
     <row r="7" spans="1:2" ht="75" x14ac:dyDescent="0.25">
-      <c r="A7" s="67" t="s">
+      <c r="A7" s="43" t="s">
         <v>45</v>
       </c>
-      <c r="B7" s="73" t="s">
+      <c r="B7" s="49" t="s">
         <v>213</v>
       </c>
     </row>
     <row r="8" spans="1:2" ht="75" x14ac:dyDescent="0.25">
-      <c r="A8" s="67" t="s">
+      <c r="A8" s="43" t="s">
         <v>97</v>
       </c>
-      <c r="B8" s="73" t="s">
+      <c r="B8" s="49" t="s">
         <v>214</v>
       </c>
     </row>
     <row r="9" spans="1:2" ht="75" x14ac:dyDescent="0.25">
-      <c r="A9" s="67" t="s">
+      <c r="A9" s="43" t="s">
         <v>42</v>
       </c>
-      <c r="B9" s="73" t="s">
+      <c r="B9" s="49" t="s">
         <v>215</v>
       </c>
     </row>
     <row r="10" spans="1:2" ht="75" x14ac:dyDescent="0.25">
-      <c r="A10" s="67" t="s">
+      <c r="A10" s="43" t="s">
         <v>89</v>
       </c>
-      <c r="B10" s="73" t="s">
+      <c r="B10" s="49" t="s">
         <v>216</v>
       </c>
     </row>

</xml_diff>